<commit_message>
Manuel Mariscal, P1838 e Ilse
</commit_message>
<xml_diff>
--- a/Proyectos/2016/6/P1727 - Servicio Integral de Ventas, Ilse Ponce Ramos _RN/Ventas/0. - Checklist 1er Curso Ilse Ponce - AGO16.xlsx
+++ b/Proyectos/2016/6/P1727 - Servicio Integral de Ventas, Ilse Ponce Ramos _RN/Ventas/0. - Checklist 1er Curso Ilse Ponce - AGO16.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Checklist Curso (2)" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Checklist Curso'!$B$5:$B$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Checklist Curso'!$B$5:$B$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Checklist Curso (2)'!$B$5:$B$45</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="84">
   <si>
     <t>a</t>
   </si>
@@ -205,9 +205,6 @@
     <t>Ilse Ponce</t>
   </si>
   <si>
-    <t>1 cte, 30% comisión, 2 o 3, 40% + 4, 50%</t>
-  </si>
-  <si>
     <t>Presupuesto</t>
   </si>
   <si>
@@ -254,6 +251,33 @@
   </si>
   <si>
     <t>Especialista</t>
+  </si>
+  <si>
+    <t>Definición de cuántas fechas y las fechas</t>
+  </si>
+  <si>
+    <t>Cuota establecida $80,000 depositados.</t>
+  </si>
+  <si>
+    <t>Preparación  de cobro  con tarjetas a través de SOS Software</t>
+  </si>
+  <si>
+    <t>CV Experto fiscalista</t>
+  </si>
+  <si>
+    <t>SOS</t>
+  </si>
+  <si>
+    <t>Evoca y Coffee Break</t>
+  </si>
+  <si>
+    <t>Listo</t>
+  </si>
+  <si>
+    <t>Kit de Marketing para Alianzas</t>
+  </si>
+  <si>
+    <t>1 cte, 30% comisión, 2 o 3, 40% + 4, 50%; especificar que en pagos con tarjeta será cobrado por SOS Software SA de CV</t>
   </si>
 </sst>
 </file>
@@ -958,8 +982,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B5:H44" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="B5:H44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B5:H45" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="B5:H45"/>
   <tableColumns count="7">
     <tableColumn id="1" name="¿Finalizada?" dataDxfId="15"/>
     <tableColumn id="9" name="Req." dataDxfId="14"/>
@@ -1277,10 +1301,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1297,7 +1321,7 @@
     <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30">
+    <row r="1" spans="1:10" ht="30">
       <c r="B1" s="11" t="s">
         <v>46</v>
       </c>
@@ -1306,20 +1330,20 @@
       <c r="E1" s="10"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="12.75">
+    <row r="2" spans="1:10" ht="12.75">
       <c r="B2" s="13"/>
       <c r="C2" s="12"/>
       <c r="F2" s="10"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:10">
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="20.25">
+    <row r="4" spans="1:10" ht="20.25">
       <c r="B4" s="17"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" ht="12.75">
+    <row r="5" spans="1:10" s="3" customFormat="1" ht="12.75">
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1342,7 +1366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="20.25">
+    <row r="6" spans="1:10" ht="20.25">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1362,7 +1386,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="20.25">
+    <row r="7" spans="1:10" ht="20.25">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -1384,7 +1408,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="20.25">
+    <row r="8" spans="1:10" ht="20.25">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -1402,7 +1426,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="21"/>
     </row>
-    <row r="9" spans="1:11" ht="20.25">
+    <row r="9" spans="1:10" ht="20.25">
       <c r="A9" s="2">
         <v>4</v>
       </c>
@@ -1422,7 +1446,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="20.25">
+    <row r="10" spans="1:10" ht="20.25">
       <c r="A10" s="2">
         <v>5</v>
       </c>
@@ -1443,12 +1467,9 @@
       <c r="H10" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="37">
-        <f>10*750*8</f>
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="39.75">
+      <c r="J10" s="37"/>
+    </row>
+    <row r="11" spans="1:10" ht="39.75">
       <c r="A11" s="2">
         <v>6</v>
       </c>
@@ -1469,12 +1490,9 @@
       <c r="H11" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="37">
-        <f>+J10*2</f>
-        <v>120000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="20.25">
+      <c r="J11" s="37"/>
+    </row>
+    <row r="12" spans="1:10" ht="20.25">
       <c r="A12" s="2">
         <v>7</v>
       </c>
@@ -1493,11 +1511,9 @@
       <c r="F12" s="7"/>
       <c r="G12" s="6"/>
       <c r="H12" s="21"/>
-      <c r="J12" s="37">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="20.25">
+      <c r="J12" s="37"/>
+    </row>
+    <row r="13" spans="1:10" ht="20.25">
       <c r="A13" s="2">
         <v>8</v>
       </c>
@@ -1515,7 +1531,7 @@
       <c r="G13" s="6"/>
       <c r="H13" s="21"/>
     </row>
-    <row r="14" spans="1:11" ht="20.25">
+    <row r="14" spans="1:10" ht="20.25">
       <c r="A14" s="2">
         <v>9</v>
       </c>
@@ -1531,17 +1547,11 @@
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="31"/>
-      <c r="J14" s="2">
-        <f>250*3</f>
-        <v>750</v>
-      </c>
-      <c r="K14" s="2">
-        <f>+J14*8</f>
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="27">
+      <c r="H14" s="31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="27">
       <c r="A15" s="2">
         <v>10</v>
       </c>
@@ -1561,7 +1571,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="20.25">
+    <row r="16" spans="1:10" ht="20.25">
       <c r="A16" s="2">
         <v>11</v>
       </c>
@@ -1578,10 +1588,6 @@
       <c r="F16" s="7"/>
       <c r="G16" s="6"/>
       <c r="H16" s="21"/>
-      <c r="J16" s="2">
-        <f>30000/75000</f>
-        <v>0.4</v>
-      </c>
     </row>
     <row r="17" spans="1:8" ht="20.25">
       <c r="A17" s="2">
@@ -1785,35 +1791,25 @@
         <v>19</v>
       </c>
       <c r="B29" s="9"/>
-      <c r="C29" s="29" t="s">
-        <v>40</v>
-      </c>
+      <c r="C29" s="29"/>
       <c r="D29" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>36</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="E29" s="19"/>
       <c r="F29" s="7"/>
-      <c r="G29" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="H29" s="21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="20.25">
+      <c r="G29" s="28"/>
+      <c r="H29" s="21"/>
+    </row>
+    <row r="30" spans="1:8" ht="39.75">
       <c r="A30" s="2">
         <v>20</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>49</v>
-      </c>
+      <c r="B30" s="9"/>
       <c r="C30" s="29" t="s">
         <v>40</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="E30" s="19" t="s">
         <v>36</v>
@@ -1823,44 +1819,58 @@
         <v>43</v>
       </c>
       <c r="H30" s="21" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="20.25">
       <c r="A31" s="2">
         <v>21</v>
       </c>
-      <c r="B31" s="9"/>
+      <c r="B31" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="C31" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>44</v>
+      <c r="D31" s="20" t="s">
+        <v>34</v>
       </c>
       <c r="E31" s="19" t="s">
         <v>36</v>
       </c>
       <c r="F31" s="7"/>
-      <c r="G31" s="6"/>
+      <c r="G31" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="H31" s="21" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="20.25">
       <c r="A32" s="2">
         <v>22</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="22" t="s">
-        <v>23</v>
+      <c r="B32" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="21"/>
+        <v>36</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G32" s="28">
+        <v>42586</v>
+      </c>
+      <c r="H32" s="21" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="33" spans="1:8" ht="20.25">
       <c r="A33" s="2">
@@ -1870,60 +1880,68 @@
         <v>0</v>
       </c>
       <c r="C33" s="29"/>
-      <c r="D33" s="24" t="s">
-        <v>24</v>
+      <c r="D33" s="22" t="s">
+        <v>23</v>
       </c>
       <c r="E33" s="19" t="s">
         <v>37</v>
       </c>
       <c r="F33" s="7"/>
-      <c r="G33" s="28">
-        <v>42551</v>
-      </c>
-      <c r="H33" s="21" t="s">
-        <v>22</v>
-      </c>
+      <c r="G33" s="6"/>
+      <c r="H33" s="21"/>
     </row>
     <row r="34" spans="1:8" ht="20.25">
       <c r="A34" s="2">
         <v>24</v>
       </c>
-      <c r="B34" s="9"/>
+      <c r="B34" s="9" t="s">
+        <v>0</v>
+      </c>
       <c r="C34" s="29"/>
       <c r="D34" s="24" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E34" s="19" t="s">
         <v>37</v>
       </c>
       <c r="F34" s="7"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="21"/>
+      <c r="G34" s="28">
+        <v>42551</v>
+      </c>
+      <c r="H34" s="21" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="35" spans="1:8" ht="20.25">
       <c r="A35" s="2">
         <v>25</v>
       </c>
-      <c r="B35" s="9"/>
+      <c r="B35" s="9" t="s">
+        <v>0</v>
+      </c>
       <c r="C35" s="29"/>
-      <c r="D35" s="22" t="s">
-        <v>25</v>
+      <c r="D35" s="24" t="s">
+        <v>8</v>
       </c>
       <c r="E35" s="19" t="s">
         <v>37</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="6"/>
-      <c r="H35" s="21"/>
+      <c r="H35" s="21" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="36" spans="1:8" ht="20.25">
       <c r="A36" s="2">
         <v>26</v>
       </c>
-      <c r="B36" s="9"/>
+      <c r="B36" s="9" t="s">
+        <v>0</v>
+      </c>
       <c r="C36" s="29"/>
-      <c r="D36" s="20" t="s">
-        <v>27</v>
+      <c r="D36" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="E36" s="19" t="s">
         <v>37</v>
@@ -1936,31 +1954,37 @@
       <c r="A37" s="2">
         <v>27</v>
       </c>
-      <c r="B37" s="9"/>
+      <c r="B37" s="9" t="s">
+        <v>0</v>
+      </c>
       <c r="C37" s="29"/>
-      <c r="D37" s="24" t="s">
-        <v>26</v>
+      <c r="D37" s="20" t="s">
+        <v>27</v>
       </c>
       <c r="E37" s="19" t="s">
         <v>37</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="21"/>
+      <c r="H37" s="21" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="38" spans="1:8" ht="20.25">
       <c r="A38" s="2">
         <v>28</v>
       </c>
-      <c r="B38" s="9"/>
+      <c r="B38" s="9" t="s">
+        <v>0</v>
+      </c>
       <c r="C38" s="29"/>
-      <c r="D38" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E38" s="19"/>
-      <c r="F38" s="7" t="s">
-        <v>58</v>
-      </c>
+      <c r="D38" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F38" s="7"/>
       <c r="G38" s="6"/>
       <c r="H38" s="21"/>
     </row>
@@ -1971,10 +1995,12 @@
       <c r="B39" s="9"/>
       <c r="C39" s="29"/>
       <c r="D39" s="6" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E39" s="19"/>
-      <c r="F39" s="7"/>
+      <c r="F39" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="G39" s="6"/>
       <c r="H39" s="21"/>
     </row>
@@ -1985,10 +2011,12 @@
       <c r="B40" s="9"/>
       <c r="C40" s="29"/>
       <c r="D40" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E40" s="19"/>
-      <c r="F40" s="7"/>
+      <c r="F40" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="G40" s="6"/>
       <c r="H40" s="21"/>
     </row>
@@ -1998,21 +2026,29 @@
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="29"/>
-      <c r="D41" s="6"/>
+      <c r="D41" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="E41" s="19"/>
-      <c r="F41" s="7"/>
+      <c r="F41" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="G41" s="6"/>
       <c r="H41" s="21"/>
     </row>
-    <row r="42" spans="1:8" ht="20.25">
+    <row r="42" spans="1:8" ht="27">
       <c r="A42" s="2">
         <v>32</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="29"/>
-      <c r="D42" s="6"/>
+      <c r="D42" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="E42" s="19"/>
-      <c r="F42" s="7"/>
+      <c r="F42" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="G42" s="6"/>
       <c r="H42" s="21"/>
     </row>
@@ -2022,9 +2058,13 @@
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="29"/>
-      <c r="D43" s="6"/>
+      <c r="D43" s="6" t="s">
+        <v>78</v>
+      </c>
       <c r="E43" s="19"/>
-      <c r="F43" s="7"/>
+      <c r="F43" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="G43" s="6"/>
       <c r="H43" s="21"/>
     </row>
@@ -2032,17 +2072,26 @@
       <c r="B44" s="9"/>
       <c r="C44" s="29"/>
       <c r="D44" s="6"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="21"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="6"/>
       <c r="H44" s="21"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" ht="20.25">
       <c r="B45" s="9"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="15"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="B46" s="9"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2072,17 +2121,17 @@
   <sheetData>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="C3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="39">
         <v>6000</v>
@@ -2090,7 +2139,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="39">
         <v>4550</v>
@@ -2098,13 +2147,13 @@
     </row>
     <row r="6" spans="1:3">
       <c r="B6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="39"/>
     </row>
     <row r="7" spans="1:3">
       <c r="B7" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" s="39">
         <v>400</v>
@@ -2112,7 +2161,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="B8" s="38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" s="39">
         <v>3000</v>
@@ -2130,13 +2179,13 @@
     </row>
     <row r="11" spans="1:3">
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="39"/>
     </row>
     <row r="12" spans="1:3">
       <c r="B12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" s="39">
         <f>20*20*8</f>
@@ -2145,13 +2194,13 @@
     </row>
     <row r="13" spans="1:3">
       <c r="B13" s="38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="40"/>
     </row>
     <row r="14" spans="1:3">
       <c r="B14" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14" s="39">
         <v>15000</v>
@@ -2159,7 +2208,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="B15" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" s="39">
         <v>5000</v>
@@ -2173,13 +2222,13 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" s="39"/>
     </row>
     <row r="19" spans="1:3">
       <c r="B19" s="38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="39">
         <v>8000</v>

</xml_diff>